<commit_message>
Analysis of MSM only dataset
</commit_message>
<xml_diff>
--- a/thresholdstats_wo_MSM.xlsx
+++ b/thresholdstats_wo_MSM.xlsx
@@ -574,7 +574,7 @@
         <v>2</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -583,7 +583,7 @@
         <v>8</v>
       </c>
       <c r="J2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K2">
         <v>69</v>
@@ -672,7 +672,7 @@
         <v>8</v>
       </c>
       <c r="J3">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K3">
         <v>118</v>
@@ -705,7 +705,7 @@
         <v>196</v>
       </c>
       <c r="U3">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V3">
         <v>3</v>
@@ -761,7 +761,7 @@
         <v>12</v>
       </c>
       <c r="J4">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K4">
         <v>160</v>
@@ -794,7 +794,7 @@
         <v>249</v>
       </c>
       <c r="U4">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="V4">
         <v>5</v>
@@ -826,7 +826,7 @@
         <v>2019</v>
       </c>
       <c r="B5">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -841,7 +841,7 @@
         <v>6</v>
       </c>
       <c r="G5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -850,16 +850,16 @@
         <v>12</v>
       </c>
       <c r="J5">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K5">
         <v>179</v>
       </c>
       <c r="L5">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="M5">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="N5">
         <v>1315</v>
@@ -874,16 +874,16 @@
         <v>1359</v>
       </c>
       <c r="R5">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="S5">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="T5">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="U5">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="V5">
         <v>5</v>
@@ -915,7 +915,7 @@
         <v>2020</v>
       </c>
       <c r="B6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -930,7 +930,7 @@
         <v>6</v>
       </c>
       <c r="G6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H6">
         <v>2</v>
@@ -939,16 +939,16 @@
         <v>13</v>
       </c>
       <c r="J6">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K6">
         <v>194</v>
       </c>
       <c r="L6">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="M6">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="N6">
         <v>1417</v>
@@ -963,16 +963,16 @@
         <v>1468</v>
       </c>
       <c r="R6">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="S6">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="T6">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="U6">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V6">
         <v>5</v>
@@ -1004,7 +1004,7 @@
         <v>2021</v>
       </c>
       <c r="B7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1019,7 +1019,7 @@
         <v>6</v>
       </c>
       <c r="G7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H7">
         <v>2</v>
@@ -1028,16 +1028,16 @@
         <v>13</v>
       </c>
       <c r="J7">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K7">
         <v>194</v>
       </c>
       <c r="L7">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="M7">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="N7">
         <v>1417</v>
@@ -1052,16 +1052,16 @@
         <v>1468</v>
       </c>
       <c r="R7">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="S7">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="T7">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="U7">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V7">
         <v>5</v>
@@ -1204,7 +1204,7 @@
         <v>3</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G2">
         <v>9</v>
@@ -1216,13 +1216,13 @@
         <v>13</v>
       </c>
       <c r="J2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K2">
         <v>108</v>
       </c>
       <c r="L2">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="M2">
         <v>303</v>
@@ -1293,7 +1293,7 @@
         <v>3</v>
       </c>
       <c r="F3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G3">
         <v>10</v>
@@ -1305,13 +1305,13 @@
         <v>15</v>
       </c>
       <c r="J3">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K3">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="L3">
-        <v>438</v>
+        <v>452</v>
       </c>
       <c r="M3">
         <v>570</v>
@@ -1335,10 +1335,10 @@
         <v>466</v>
       </c>
       <c r="T3">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="U3">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="V3">
         <v>4</v>
@@ -1382,7 +1382,7 @@
         <v>5</v>
       </c>
       <c r="F4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G4">
         <v>11</v>
@@ -1394,13 +1394,13 @@
         <v>19</v>
       </c>
       <c r="J4">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K4">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="L4">
-        <v>551</v>
+        <v>566</v>
       </c>
       <c r="M4">
         <v>723</v>
@@ -1424,10 +1424,10 @@
         <v>591</v>
       </c>
       <c r="T4">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="U4">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="V4">
         <v>7</v>
@@ -1459,7 +1459,7 @@
         <v>2019</v>
       </c>
       <c r="B5">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1471,10 +1471,10 @@
         <v>5</v>
       </c>
       <c r="F5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -1483,13 +1483,13 @@
         <v>20</v>
       </c>
       <c r="J5">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K5">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="L5">
-        <v>650</v>
+        <v>666</v>
       </c>
       <c r="M5">
         <v>875</v>
@@ -1513,10 +1513,10 @@
         <v>710</v>
       </c>
       <c r="T5">
-        <v>388</v>
+        <v>396</v>
       </c>
       <c r="U5">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="V5">
         <v>7</v>
@@ -1548,7 +1548,7 @@
         <v>2020</v>
       </c>
       <c r="B6">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1560,10 +1560,10 @@
         <v>6</v>
       </c>
       <c r="F6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H6">
         <v>2</v>
@@ -1572,13 +1572,13 @@
         <v>22</v>
       </c>
       <c r="J6">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K6">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="L6">
-        <v>702</v>
+        <v>718</v>
       </c>
       <c r="M6">
         <v>955</v>
@@ -1602,10 +1602,10 @@
         <v>769</v>
       </c>
       <c r="T6">
-        <v>418</v>
+        <v>426</v>
       </c>
       <c r="U6">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="V6">
         <v>9</v>
@@ -1637,7 +1637,7 @@
         <v>2021</v>
       </c>
       <c r="B7">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1649,10 +1649,10 @@
         <v>6</v>
       </c>
       <c r="F7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G7">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H7">
         <v>2</v>
@@ -1661,13 +1661,13 @@
         <v>22</v>
       </c>
       <c r="J7">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K7">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="L7">
-        <v>702</v>
+        <v>718</v>
       </c>
       <c r="M7">
         <v>955</v>
@@ -1691,10 +1691,10 @@
         <v>769</v>
       </c>
       <c r="T7">
-        <v>418</v>
+        <v>426</v>
       </c>
       <c r="U7">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="V7">
         <v>9</v>
@@ -1849,7 +1849,7 @@
         <v>25</v>
       </c>
       <c r="J2">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K2">
         <v>126</v>
@@ -1938,7 +1938,7 @@
         <v>36</v>
       </c>
       <c r="J3">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K3">
         <v>211</v>
@@ -2027,7 +2027,7 @@
         <v>45</v>
       </c>
       <c r="J4">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K4">
         <v>259</v>
@@ -2092,7 +2092,7 @@
         <v>2019</v>
       </c>
       <c r="B5">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -2107,7 +2107,7 @@
         <v>19</v>
       </c>
       <c r="G5">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5">
         <v>6</v>
@@ -2116,16 +2116,16 @@
         <v>48</v>
       </c>
       <c r="J5">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K5">
         <v>291</v>
       </c>
       <c r="L5">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="M5">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N5">
         <v>18</v>
@@ -2140,13 +2140,13 @@
         <v>0</v>
       </c>
       <c r="R5">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="S5">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="T5">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="U5">
         <v>158</v>
@@ -2181,7 +2181,7 @@
         <v>2020</v>
       </c>
       <c r="B6">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -2196,7 +2196,7 @@
         <v>19</v>
       </c>
       <c r="G6">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6">
         <v>7</v>
@@ -2205,16 +2205,16 @@
         <v>51</v>
       </c>
       <c r="J6">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K6">
         <v>305</v>
       </c>
       <c r="L6">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="M6">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="N6">
         <v>19</v>
@@ -2229,13 +2229,13 @@
         <v>0</v>
       </c>
       <c r="R6">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S6">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="T6">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="U6">
         <v>165</v>
@@ -2270,7 +2270,7 @@
         <v>2021</v>
       </c>
       <c r="B7">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -2285,7 +2285,7 @@
         <v>19</v>
       </c>
       <c r="G7">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7">
         <v>7</v>
@@ -2294,16 +2294,16 @@
         <v>51</v>
       </c>
       <c r="J7">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K7">
         <v>305</v>
       </c>
       <c r="L7">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="M7">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="N7">
         <v>19</v>
@@ -2318,13 +2318,13 @@
         <v>0</v>
       </c>
       <c r="R7">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S7">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="T7">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="U7">
         <v>165</v>
@@ -2482,13 +2482,13 @@
         <v>25</v>
       </c>
       <c r="J2">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K2">
         <v>94</v>
       </c>
       <c r="L2">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M2">
         <v>9</v>
@@ -2571,13 +2571,13 @@
         <v>35</v>
       </c>
       <c r="J3">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K3">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="L3">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="M3">
         <v>24</v>
@@ -2601,10 +2601,10 @@
         <v>44</v>
       </c>
       <c r="T3">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="U3">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="V3">
         <v>24</v>
@@ -2660,13 +2660,13 @@
         <v>43</v>
       </c>
       <c r="J4">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K4">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="L4">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="M4">
         <v>42</v>
@@ -2690,10 +2690,10 @@
         <v>65</v>
       </c>
       <c r="T4">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="U4">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="V4">
         <v>25</v>
@@ -2725,7 +2725,7 @@
         <v>2019</v>
       </c>
       <c r="B5">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -2740,7 +2740,7 @@
         <v>19</v>
       </c>
       <c r="G5">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5">
         <v>6</v>
@@ -2749,13 +2749,13 @@
         <v>46</v>
       </c>
       <c r="J5">
+        <v>123</v>
+      </c>
+      <c r="K5">
+        <v>202</v>
+      </c>
+      <c r="L5">
         <v>124</v>
-      </c>
-      <c r="K5">
-        <v>210</v>
-      </c>
-      <c r="L5">
-        <v>149</v>
       </c>
       <c r="M5">
         <v>50</v>
@@ -2779,10 +2779,10 @@
         <v>88</v>
       </c>
       <c r="T5">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="U5">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="V5">
         <v>27</v>
@@ -2814,7 +2814,7 @@
         <v>2020</v>
       </c>
       <c r="B6">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -2829,7 +2829,7 @@
         <v>19</v>
       </c>
       <c r="G6">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6">
         <v>7</v>
@@ -2838,13 +2838,13 @@
         <v>49</v>
       </c>
       <c r="J6">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K6">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="L6">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="M6">
         <v>51</v>
@@ -2868,10 +2868,10 @@
         <v>88</v>
       </c>
       <c r="T6">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="U6">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="V6">
         <v>28</v>
@@ -2903,7 +2903,7 @@
         <v>2021</v>
       </c>
       <c r="B7">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -2918,7 +2918,7 @@
         <v>19</v>
       </c>
       <c r="G7">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H7">
         <v>7</v>
@@ -2927,13 +2927,13 @@
         <v>49</v>
       </c>
       <c r="J7">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K7">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="L7">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="M7">
         <v>51</v>
@@ -2957,10 +2957,10 @@
         <v>88</v>
       </c>
       <c r="T7">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="U7">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="V7">
         <v>28</v>
@@ -3106,7 +3106,7 @@
         <v>2</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -3115,7 +3115,7 @@
         <v>8</v>
       </c>
       <c r="J2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K2">
         <v>69</v>
@@ -3237,7 +3237,7 @@
         <v>101</v>
       </c>
       <c r="U3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="V3">
         <v>3</v>
@@ -3358,7 +3358,7 @@
         <v>2019</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3373,7 +3373,7 @@
         <v>3</v>
       </c>
       <c r="G5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -3388,10 +3388,10 @@
         <v>42</v>
       </c>
       <c r="L5">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="M5">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="N5">
         <v>210</v>
@@ -3406,13 +3406,13 @@
         <v>206</v>
       </c>
       <c r="R5">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="S5">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="T5">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U5">
         <v>19</v>
@@ -3736,7 +3736,7 @@
         <v>3</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G2">
         <v>9</v>
@@ -3748,13 +3748,13 @@
         <v>13</v>
       </c>
       <c r="J2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K2">
         <v>108</v>
       </c>
       <c r="L2">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="M2">
         <v>303</v>
@@ -3825,7 +3825,7 @@
         <v>3</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G3">
         <v>6</v>
@@ -3840,10 +3840,10 @@
         <v>31</v>
       </c>
       <c r="K3">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="L3">
-        <v>220</v>
+        <v>233</v>
       </c>
       <c r="M3">
         <v>290</v>
@@ -3867,10 +3867,10 @@
         <v>245</v>
       </c>
       <c r="T3">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="U3">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="V3">
         <v>3</v>
@@ -3929,10 +3929,10 @@
         <v>34</v>
       </c>
       <c r="K4">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="L4">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="M4">
         <v>173</v>
@@ -3956,10 +3956,10 @@
         <v>158</v>
       </c>
       <c r="T4">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="U4">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="V4">
         <v>6</v>
@@ -3991,7 +3991,7 @@
         <v>2019</v>
       </c>
       <c r="B5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -4006,7 +4006,7 @@
         <v>6</v>
       </c>
       <c r="G5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -4021,7 +4021,7 @@
         <v>55</v>
       </c>
       <c r="L5">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="M5">
         <v>161</v>
@@ -4045,7 +4045,7 @@
         <v>134</v>
       </c>
       <c r="T5">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="U5">
         <v>28</v>
@@ -4381,7 +4381,7 @@
         <v>25</v>
       </c>
       <c r="J2">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K2">
         <v>126</v>
@@ -4624,7 +4624,7 @@
         <v>2019</v>
       </c>
       <c r="B5">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -4639,7 +4639,7 @@
         <v>10</v>
       </c>
       <c r="G5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5">
         <v>3</v>
@@ -4654,10 +4654,10 @@
         <v>60</v>
       </c>
       <c r="L5">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M5">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -4672,13 +4672,13 @@
         <v>0</v>
       </c>
       <c r="R5">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S5">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T5">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="U5">
         <v>44</v>
@@ -5014,13 +5014,13 @@
         <v>25</v>
       </c>
       <c r="J2">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K2">
         <v>94</v>
       </c>
       <c r="L2">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M2">
         <v>9</v>
@@ -5106,10 +5106,10 @@
         <v>59</v>
       </c>
       <c r="K3">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="L3">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="M3">
         <v>15</v>
@@ -5133,10 +5133,10 @@
         <v>33</v>
       </c>
       <c r="T3">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="U3">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="V3">
         <v>15</v>
@@ -5195,10 +5195,10 @@
         <v>39</v>
       </c>
       <c r="K4">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L4">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="M4">
         <v>19</v>
@@ -5222,7 +5222,7 @@
         <v>26</v>
       </c>
       <c r="T4">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="U4">
         <v>44</v>
@@ -5257,7 +5257,7 @@
         <v>2019</v>
       </c>
       <c r="B5">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -5272,7 +5272,7 @@
         <v>10</v>
       </c>
       <c r="G5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5">
         <v>3</v>
@@ -5287,7 +5287,7 @@
         <v>44</v>
       </c>
       <c r="L5">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M5">
         <v>8</v>
@@ -5311,7 +5311,7 @@
         <v>28</v>
       </c>
       <c r="T5">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U5">
         <v>39</v>

</xml_diff>